<commit_message>
refactored performance early stop
</commit_message>
<xml_diff>
--- a/tests/test_data/test_performance_observer_cost.xlsx
+++ b/tests/test_data/test_performance_observer_cost.xlsx
@@ -461,7 +461,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q15" sqref="Q15"/>
+      <selection activeCell="H4" sqref="H4:H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -519,7 +519,7 @@
         <v>0.01</v>
       </c>
       <c r="H2" t="b">
-        <f>IF(F2&gt;=patience,TRUE)</f>
+        <f>IF(F2=patience-1,TRUE)</f>
         <v>0</v>
       </c>
       <c r="I2">
@@ -537,7 +537,7 @@
         <v>9.9</v>
       </c>
       <c r="C3">
-        <f>IF(D3&gt;epsilon,B2,C2)</f>
+        <f>IF(H3=TRUE,B3,IF(D3&gt;epsilon,B3,C2))</f>
         <v>10</v>
       </c>
       <c r="D3">
@@ -549,36 +549,36 @@
         <v>0</v>
       </c>
       <c r="F3">
-        <f>IF(E3=TRUE,0,F2+1)</f>
+        <f>IF(E3=TRUE,0,MOD(F2+1,5))</f>
         <v>1</v>
       </c>
       <c r="G3">
         <v>0.01</v>
       </c>
       <c r="H3" t="b">
-        <f>IF(F3&gt;=patience,TRUE)</f>
+        <f>IF(F2=patience-1,TRUE)</f>
         <v>0</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I21" si="1">IF(D3&gt;epsilon,A3,I2)</f>
+        <f>IF(C3&lt;&gt;C2,A3,I2)</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f t="shared" ref="A4:A21" si="2">A3+1</f>
+        <f t="shared" ref="A4:A21" si="1">A3+1</f>
         <v>2</v>
       </c>
       <c r="B4">
-        <f t="shared" ref="B4:B21" si="3">B3-(B3*G3)</f>
+        <f t="shared" ref="B4:B21" si="2">B3-(B3*G3)</f>
         <v>9.8010000000000002</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:C21" si="4">IF(D4&gt;epsilon,B4,C3)</f>
+        <f>IF(H4=TRUE,B4,IF(D4&gt;epsilon,B4,C3))</f>
         <v>10</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D21" si="5">(C3-B4)/C3</f>
+        <f t="shared" ref="D4:D21" si="3">(C3-B4)/C3</f>
         <v>1.9899999999999984E-2</v>
       </c>
       <c r="E4" t="b">
@@ -586,36 +586,36 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <f t="shared" ref="F4:F21" si="6">IF(E4=TRUE,0,F3+1)</f>
+        <f t="shared" ref="F4:F21" si="4">IF(E4=TRUE,0,MOD(F3+1,5))</f>
         <v>2</v>
       </c>
       <c r="G4">
         <v>0.01</v>
       </c>
       <c r="H4" t="b">
-        <f>IF(F4&gt;=patience,TRUE)</f>
+        <f>IF(F3=patience-1,TRUE)</f>
         <v>0</v>
       </c>
       <c r="I4">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="I4:I21" si="5">IF(C4&lt;&gt;C3,A4,I3)</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="B5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>9.7029899999999998</v>
       </c>
       <c r="C5">
-        <f t="shared" si="4"/>
+        <f>IF(H5=TRUE,B5,IF(D5&gt;epsilon,B5,C4))</f>
         <v>9.7029899999999998</v>
       </c>
       <c r="D5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>2.9701000000000023E-2</v>
       </c>
       <c r="E5" t="b">
@@ -623,36 +623,36 @@
         <v>1</v>
       </c>
       <c r="F5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G5">
         <v>0.01</v>
       </c>
       <c r="H5" t="b">
-        <f>IF(F5&gt;=patience,TRUE)</f>
+        <f>IF(F4=patience-1,TRUE)</f>
         <v>0</v>
       </c>
       <c r="I5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="B6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>9.605960099999999</v>
       </c>
       <c r="C6">
-        <f t="shared" si="4"/>
+        <f>IF(H6=TRUE,B6,IF(D6&gt;epsilon,B6,C5))</f>
         <v>9.7029899999999998</v>
       </c>
       <c r="D6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>1.000000000000008E-2</v>
       </c>
       <c r="E6" t="b">
@@ -660,36 +660,36 @@
         <v>0</v>
       </c>
       <c r="F6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="G6">
         <v>0.01</v>
       </c>
       <c r="H6" t="b">
-        <f>IF(F6&gt;=patience,TRUE)</f>
+        <f>IF(F5=patience-1,TRUE)</f>
         <v>0</v>
       </c>
       <c r="I6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="B7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>9.5099004989999987</v>
       </c>
       <c r="C7">
-        <f t="shared" si="4"/>
+        <f>IF(H7=TRUE,B7,IF(D7&gt;epsilon,B7,C6))</f>
         <v>9.7029899999999998</v>
       </c>
       <c r="D7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>1.9900000000000116E-2</v>
       </c>
       <c r="E7" t="b">
@@ -697,37 +697,37 @@
         <v>0</v>
       </c>
       <c r="F7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="G7">
-        <f t="shared" ref="G7:G12" si="7">epsilon/10</f>
+        <f t="shared" ref="G7:G12" si="6">epsilon/10</f>
         <v>2E-3</v>
       </c>
       <c r="H7" t="b">
-        <f>IF(F7&gt;=patience,TRUE)</f>
+        <f>IF(F6=patience-1,TRUE)</f>
         <v>0</v>
       </c>
       <c r="I7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="B8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>9.4908806980019982</v>
       </c>
       <c r="C8">
-        <f t="shared" si="4"/>
+        <f>IF(H8=TRUE,B8,IF(D8&gt;epsilon,B8,C7))</f>
         <v>9.4908806980019982</v>
       </c>
       <c r="D8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>2.1860200000000166E-2</v>
       </c>
       <c r="E8" t="b">
@@ -735,37 +735,37 @@
         <v>1</v>
       </c>
       <c r="F8">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G8">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <f t="shared" si="7"/>
         <v>2E-3</v>
       </c>
       <c r="H8" t="b">
-        <f>IF(F8&gt;=patience,TRUE)</f>
+        <f>IF(F7=patience-1,TRUE)</f>
         <v>0</v>
       </c>
       <c r="I8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="B9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>9.471898936605994</v>
       </c>
       <c r="C9">
-        <f t="shared" si="4"/>
+        <f>IF(H9=TRUE,B9,IF(D9&gt;epsilon,B9,C8))</f>
         <v>9.4908806980019982</v>
       </c>
       <c r="D9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>2.0000000000000174E-3</v>
       </c>
       <c r="E9" t="b">
@@ -773,37 +773,37 @@
         <v>0</v>
       </c>
       <c r="F9">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="G9">
         <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="G9">
-        <f t="shared" si="7"/>
         <v>2E-3</v>
       </c>
       <c r="H9" t="b">
-        <f>IF(F9&gt;=patience,TRUE)</f>
+        <f>IF(F8=patience-1,TRUE)</f>
         <v>0</v>
       </c>
       <c r="I9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="B10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>9.4529551387327828</v>
       </c>
       <c r="C10">
-        <f t="shared" si="4"/>
+        <f>IF(H10=TRUE,B10,IF(D10&gt;epsilon,B10,C9))</f>
         <v>9.4908806980019982</v>
       </c>
       <c r="D10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>3.9959999999999354E-3</v>
       </c>
       <c r="E10" t="b">
@@ -811,37 +811,37 @@
         <v>0</v>
       </c>
       <c r="F10">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="G10">
         <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="G10">
-        <f t="shared" si="7"/>
         <v>2E-3</v>
       </c>
       <c r="H10" t="b">
-        <f>IF(F10&gt;=patience,TRUE)</f>
+        <f>IF(F9=patience-1,TRUE)</f>
         <v>0</v>
       </c>
       <c r="I10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="B11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>9.4340492284553168</v>
       </c>
       <c r="C11">
-        <f t="shared" si="4"/>
+        <f>IF(H11=TRUE,B11,IF(D11&gt;epsilon,B11,C10))</f>
         <v>9.4908806980019982</v>
       </c>
       <c r="D11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>5.988007999999983E-3</v>
       </c>
       <c r="E11" t="b">
@@ -849,37 +849,37 @@
         <v>0</v>
       </c>
       <c r="F11">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="G11">
         <f t="shared" si="6"/>
-        <v>3</v>
-      </c>
-      <c r="G11">
-        <f t="shared" si="7"/>
         <v>2E-3</v>
       </c>
       <c r="H11" t="b">
-        <f>IF(F11&gt;=patience,TRUE)</f>
+        <f>IF(F10=patience-1,TRUE)</f>
         <v>0</v>
       </c>
       <c r="I11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="B12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>9.4151811299984054</v>
       </c>
       <c r="C12">
-        <f t="shared" si="4"/>
+        <f>IF(H12=TRUE,B12,IF(D12&gt;epsilon,B12,C11))</f>
         <v>9.4908806980019982</v>
       </c>
       <c r="D12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>7.9760319840000635E-3</v>
       </c>
       <c r="E12" t="b">
@@ -887,37 +887,37 @@
         <v>0</v>
       </c>
       <c r="F12">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="G12">
         <f t="shared" si="6"/>
-        <v>4</v>
-      </c>
-      <c r="G12">
-        <f t="shared" si="7"/>
         <v>2E-3</v>
       </c>
       <c r="H12" t="b">
-        <f>IF(F12&gt;=patience,TRUE)</f>
+        <f>IF(F11=patience-1,TRUE)</f>
         <v>0</v>
       </c>
       <c r="I12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="B13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>9.3963507677384079</v>
       </c>
       <c r="C13">
-        <f t="shared" si="4"/>
-        <v>9.4908806980019982</v>
+        <f>IF(H13=TRUE,B13,IF(D13&gt;epsilon,B13,C12))</f>
+        <v>9.3963507677384079</v>
       </c>
       <c r="D13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>9.9600799200321322E-3</v>
       </c>
       <c r="E13" t="b">
@@ -925,315 +925,315 @@
         <v>0</v>
       </c>
       <c r="F13">
-        <f t="shared" si="6"/>
-        <v>5</v>
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
       <c r="G13">
         <v>1E-3</v>
       </c>
       <c r="H13" t="b">
-        <f>IF(F13&gt;=patience,TRUE)</f>
+        <f>IF(F12=patience-1,TRUE)</f>
         <v>1</v>
       </c>
       <c r="I13">
-        <f t="shared" si="1"/>
-        <v>6</v>
+        <f t="shared" si="5"/>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="B14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>9.3869544169706689</v>
       </c>
       <c r="C14">
-        <f t="shared" si="4"/>
-        <v>9.4908806980019982</v>
+        <f>IF(H14=TRUE,B14,IF(D14&gt;epsilon,B14,C13))</f>
+        <v>9.3963507677384079</v>
       </c>
       <c r="D14">
-        <f t="shared" si="5"/>
-        <v>1.0950119840112165E-2</v>
+        <f t="shared" si="3"/>
+        <v>1.000000000000067E-3</v>
       </c>
       <c r="E14" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F14">
-        <f t="shared" si="6"/>
-        <v>6</v>
+        <f t="shared" si="4"/>
+        <v>1</v>
       </c>
       <c r="G14">
         <v>1E-3</v>
       </c>
       <c r="H14" t="b">
-        <f>IF(F14&gt;=patience,TRUE)</f>
-        <v>1</v>
+        <f>IF(F13=patience-1,TRUE)</f>
+        <v>0</v>
       </c>
       <c r="I14">
-        <f t="shared" si="1"/>
-        <v>6</v>
+        <f t="shared" si="5"/>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="B15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>9.3775674625536976</v>
       </c>
       <c r="C15">
-        <f t="shared" si="4"/>
-        <v>9.4908806980019982</v>
+        <f>IF(H15=TRUE,B15,IF(D15&gt;epsilon,B15,C14))</f>
+        <v>9.3963507677384079</v>
       </c>
       <c r="D15">
-        <f t="shared" si="5"/>
-        <v>1.1939169720272126E-2</v>
+        <f t="shared" si="3"/>
+        <v>1.9990000000001391E-3</v>
       </c>
       <c r="E15" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F15">
-        <f t="shared" si="6"/>
-        <v>7</v>
+        <f t="shared" si="4"/>
+        <v>2</v>
       </c>
       <c r="G15">
         <v>2E-3</v>
       </c>
       <c r="H15" t="b">
-        <f>IF(F15&gt;=patience,TRUE)</f>
-        <v>1</v>
+        <f>IF(F14=patience-1,TRUE)</f>
+        <v>0</v>
       </c>
       <c r="I15">
-        <f t="shared" si="1"/>
-        <v>6</v>
+        <f t="shared" si="5"/>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="B16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>9.3588123276285895</v>
       </c>
       <c r="C16">
-        <f t="shared" si="4"/>
-        <v>9.4908806980019982</v>
+        <f>IF(H16=TRUE,B16,IF(D16&gt;epsilon,B16,C15))</f>
+        <v>9.3963507677384079</v>
       </c>
       <c r="D16">
-        <f t="shared" si="5"/>
-        <v>1.3915291380831651E-2</v>
+        <f t="shared" si="3"/>
+        <v>3.9950020000002091E-3</v>
       </c>
       <c r="E16" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F16">
-        <f t="shared" si="6"/>
-        <v>8</v>
+        <f t="shared" si="4"/>
+        <v>3</v>
       </c>
       <c r="G16">
         <v>2E-3</v>
       </c>
       <c r="H16" t="b">
-        <f>IF(F16&gt;=patience,TRUE)</f>
-        <v>1</v>
+        <f>IF(F15=patience-1,TRUE)</f>
+        <v>0</v>
       </c>
       <c r="I16">
-        <f t="shared" si="1"/>
-        <v>6</v>
+        <f t="shared" si="5"/>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="B17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>9.3400947029733317</v>
       </c>
       <c r="C17">
-        <f t="shared" si="4"/>
-        <v>9.4908806980019982</v>
+        <f>IF(H17=TRUE,B17,IF(D17&gt;epsilon,B17,C16))</f>
+        <v>9.3963507677384079</v>
       </c>
       <c r="D17">
-        <f t="shared" si="5"/>
-        <v>1.5887460798070057E-2</v>
+        <f t="shared" si="3"/>
+        <v>5.9870119960002783E-3</v>
       </c>
       <c r="E17" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F17">
-        <f t="shared" si="6"/>
-        <v>9</v>
+        <f t="shared" si="4"/>
+        <v>4</v>
       </c>
       <c r="G17">
         <v>2E-3</v>
       </c>
       <c r="H17" t="b">
-        <f>IF(F17&gt;=patience,TRUE)</f>
-        <v>1</v>
+        <f>IF(F16=patience-1,TRUE)</f>
+        <v>0</v>
       </c>
       <c r="I17">
-        <f t="shared" si="1"/>
-        <v>6</v>
+        <f t="shared" si="5"/>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="B18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>9.3214145135673849</v>
       </c>
       <c r="C18">
-        <f t="shared" si="4"/>
-        <v>9.4908806980019982</v>
+        <f>IF(H18=TRUE,B18,IF(D18&gt;epsilon,B18,C17))</f>
+        <v>9.3214145135673849</v>
       </c>
       <c r="D18">
-        <f t="shared" si="5"/>
-        <v>1.7855685876473924E-2</v>
+        <f t="shared" si="3"/>
+        <v>7.9750379720082854E-3</v>
       </c>
       <c r="E18" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F18">
-        <f t="shared" si="6"/>
-        <v>10</v>
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
       <c r="G18">
         <v>2E-3</v>
       </c>
       <c r="H18" t="b">
-        <f>IF(F18&gt;=patience,TRUE)</f>
+        <f>IF(F17=patience-1,TRUE)</f>
         <v>1</v>
       </c>
       <c r="I18">
-        <f t="shared" si="1"/>
-        <v>6</v>
+        <f t="shared" si="5"/>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="B19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>9.3027716845402502</v>
       </c>
       <c r="C19">
-        <f t="shared" si="4"/>
-        <v>9.4908806980019982</v>
+        <f>IF(H19=TRUE,B19,IF(D19&gt;epsilon,B19,C18))</f>
+        <v>9.3214145135673849</v>
       </c>
       <c r="D19">
-        <f t="shared" si="5"/>
-        <v>1.9819974504720974E-2</v>
+        <f t="shared" si="3"/>
+        <v>1.9999999999999996E-3</v>
       </c>
       <c r="E19" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F19">
-        <f t="shared" si="6"/>
-        <v>11</v>
+        <f t="shared" si="4"/>
+        <v>1</v>
       </c>
       <c r="G19">
         <v>2E-3</v>
       </c>
       <c r="H19" t="b">
-        <f>IF(F19&gt;=patience,TRUE)</f>
-        <v>1</v>
+        <f>IF(F18=patience-1,TRUE)</f>
+        <v>0</v>
       </c>
       <c r="I19">
-        <f t="shared" si="1"/>
-        <v>6</v>
+        <f t="shared" si="5"/>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="B20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>9.2841661411711698</v>
       </c>
       <c r="C20">
-        <f t="shared" si="4"/>
-        <v>9.2841661411711698</v>
+        <f>IF(H20=TRUE,B20,IF(D20&gt;epsilon,B20,C19))</f>
+        <v>9.3214145135673849</v>
       </c>
       <c r="D20">
-        <f t="shared" si="5"/>
-        <v>2.178033455571152E-2</v>
+        <f t="shared" si="3"/>
+        <v>3.9959999999999865E-3</v>
       </c>
       <c r="E20" t="b">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F20">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>2</v>
       </c>
       <c r="G20">
         <v>2E-3</v>
       </c>
       <c r="H20" t="b">
-        <f>IF(F20&gt;=patience,TRUE)</f>
+        <f>IF(F19=patience-1,TRUE)</f>
         <v>0</v>
       </c>
       <c r="I20">
-        <f t="shared" si="1"/>
-        <v>18</v>
+        <f t="shared" si="5"/>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="B21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>9.2655978088888276</v>
       </c>
       <c r="C21">
-        <f t="shared" si="4"/>
-        <v>9.2841661411711698</v>
+        <f>IF(H21=TRUE,B21,IF(D21&gt;epsilon,B21,C20))</f>
+        <v>9.3214145135673849</v>
       </c>
       <c r="D21">
-        <f t="shared" si="5"/>
-        <v>1.9999999999999879E-3</v>
+        <f t="shared" si="3"/>
+        <v>5.9880079999999744E-3</v>
       </c>
       <c r="E21" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F21">
-        <f t="shared" si="6"/>
-        <v>1</v>
+        <f t="shared" si="4"/>
+        <v>3</v>
       </c>
       <c r="G21">
         <v>2E-3</v>
       </c>
       <c r="H21" t="b">
-        <f>IF(F21&gt;=patience,TRUE)</f>
+        <f>IF(F20=patience-1,TRUE)</f>
         <v>0</v>
       </c>
       <c r="I21">
-        <f t="shared" si="1"/>
-        <v>18</v>
+        <f t="shared" si="5"/>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removed val_cost updated summary
</commit_message>
<xml_diff>
--- a/tests/test_data/test_performance_observer_cost.xlsx
+++ b/tests/test_data/test_performance_observer_cost.xlsx
@@ -458,10 +458,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:XFD21"/>
+      <selection activeCell="H4" sqref="H4:H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -940,6 +940,302 @@
         <v>11</v>
       </c>
     </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="4"/>
+        <v>9.3869544169706689</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>9.3963507677384079</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="5"/>
+        <v>1.000000000000067E-3</v>
+      </c>
+      <c r="E14" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>1E-3</v>
+      </c>
+      <c r="H14" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="7"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="4"/>
+        <v>9.3775674625536976</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>9.3963507677384079</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="5"/>
+        <v>1.9990000000001391E-3</v>
+      </c>
+      <c r="E15" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="G15">
+        <v>2E-3</v>
+      </c>
+      <c r="H15" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="7"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="4"/>
+        <v>9.3588123276285895</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>9.3963507677384079</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="5"/>
+        <v>3.9950020000002091E-3</v>
+      </c>
+      <c r="E16" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="G16">
+        <v>2E-3</v>
+      </c>
+      <c r="H16" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="7"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="4"/>
+        <v>9.3400947029733317</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>9.3963507677384079</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="5"/>
+        <v>5.9870119960002783E-3</v>
+      </c>
+      <c r="E17" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="G17">
+        <v>2E-3</v>
+      </c>
+      <c r="H17" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="7"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="4"/>
+        <v>9.3214145135673849</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>9.3214145135673849</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="5"/>
+        <v>7.9750379720082854E-3</v>
+      </c>
+      <c r="E18" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>2E-3</v>
+      </c>
+      <c r="H18" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="7"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <f t="shared" si="3"/>
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="4"/>
+        <v>9.3027716845402502</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>9.3214145135673849</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="5"/>
+        <v>1.9999999999999996E-3</v>
+      </c>
+      <c r="E19" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>2E-3</v>
+      </c>
+      <c r="H19" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="7"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <f t="shared" si="3"/>
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="4"/>
+        <v>9.2841661411711698</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>9.3214145135673849</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="5"/>
+        <v>3.9959999999999865E-3</v>
+      </c>
+      <c r="E20" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="G20">
+        <v>2E-3</v>
+      </c>
+      <c r="H20" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="7"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <f t="shared" si="3"/>
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="4"/>
+        <v>9.2655978088888276</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>9.3214145135673849</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="5"/>
+        <v>5.9880079999999744E-3</v>
+      </c>
+      <c r="E21" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="G21">
+        <v>2E-3</v>
+      </c>
+      <c r="H21" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="7"/>
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>